<commit_message>
Revert "Revert "no message""
This reverts commit 41be4a0398690ef73bcf300e2ed091669984523b.
</commit_message>
<xml_diff>
--- a/00_WBS/スケジュール1.xlsx
+++ b/00_WBS/スケジュール1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bf4bb4a0a505561/桌面/新しいフォルダー/00_WBS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{6FED28F5-EFDF-754F-B530-AC76CEF244BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE643CB-887B-407F-AE47-B381CD56EE7F}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{6FED28F5-EFDF-754F-B530-AC76CEF244BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDD8D0FA-43E2-415C-BBA9-C6A8CA29FBB4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="52">
   <si>
     <t>勤怠管理システムWBS</t>
   </si>
@@ -199,7 +199,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm/dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,11 +271,6 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -389,7 +384,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -441,7 +436,6 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -505,7 +499,28 @@
     <cellStyle name="標準_2004.05.14_経費管理_機・一覧・" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
     <cellStyle name="標準_システム管理" xfId="1" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
-  <dxfs count="53">
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.1498764000366222"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1151,13 +1166,13 @@
   <dimension ref="B3:DB15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="6" topLeftCell="O7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L21" activeCellId="0" sqref="L21"/>
+      <selection pane="bottomRight" activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="1" outlineLevelRow="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="5" style="7" customWidth="1"/>
     <col min="2" max="2" width="4.296875" style="8" customWidth="1"/>
@@ -1165,483 +1180,402 @@
     <col min="4" max="4" width="13.19921875" style="7" customWidth="1"/>
     <col min="5" max="5" width="6.69921875" style="7" customWidth="1"/>
     <col min="6" max="6" width="10.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="11" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="9.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="18" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
     <col min="19" max="19" width="2" style="7" customWidth="1"/>
-    <col min="20" max="20" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="24" max="24" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="20" max="25" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
     <col min="26" max="26" width="9.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="32" width="6.69921875" style="7" customWidth="1" outlineLevel="1"/>
     <col min="33" max="33" width="1.69921875" style="7" customWidth="1"/>
-    <col min="34" max="34" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="37" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="39" max="39" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="41" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="42" max="42" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="43" max="43" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="46" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="47" max="47" width="1.69921875" style="7" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="50" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="51" max="51" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="52" max="52" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="54" max="54" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="55" max="55" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="59" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="60" max="60" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="48" max="60" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="61" max="61" width="1.69921875" style="7" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="64" max="64" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="65" max="65" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="66" max="66" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="67" max="67" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="68" max="68" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="69" max="69" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="70" max="70" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="71" max="71" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="72" max="72" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="73" max="73" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="74" max="74" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="75" max="75" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="75" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="76" max="76" width="1.69921875" style="7" customWidth="1" collapsed="1"/>
-    <col min="77" max="77" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="78" max="78" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="79" max="79" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="80" max="80" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="81" max="81" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="82" max="82" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="83" max="83" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="84" max="84" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="85" max="85" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="86" max="86" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="87" max="87" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="88" max="88" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="89" max="89" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="77" max="89" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="90" max="90" width="1.69921875" style="7" customWidth="1" collapsed="1"/>
-    <col min="91" max="91" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="92" max="92" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="93" max="93" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="94" max="94" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="95" max="95" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="96" max="96" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="97" max="97" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="98" max="98" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="99" max="99" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="100" max="100" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="101" max="101" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="102" max="102" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="103" max="103" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="104" max="104" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="91" max="104" width="6.69921875" style="7" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="105" max="105" width="1.69921875" style="7" customWidth="1" collapsed="1"/>
     <col min="106" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" ht="23">
+    <row r="3" spans="2:106" ht="23.4">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" ht="14">
-      <c r="B4" s="22" t="s">
+    <row r="4" spans="2:106" ht="14.4">
+      <c r="B4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24" t="s">
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="T4" s="24" t="s">
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="T4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24" t="s">
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
-      <c r="AH4" s="24" t="s">
+      <c r="AA4" s="23"/>
+      <c r="AB4" s="23"/>
+      <c r="AC4" s="23"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AH4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="24"/>
-      <c r="AK4" s="24"/>
-      <c r="AL4" s="24"/>
-      <c r="AM4" s="24"/>
-      <c r="AN4" s="24" t="s">
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="23"/>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="23"/>
+      <c r="AN4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="AO4" s="24"/>
-      <c r="AP4" s="24"/>
-      <c r="AQ4" s="24"/>
-      <c r="AR4" s="24"/>
-      <c r="AS4" s="24"/>
-      <c r="AT4" s="24"/>
-      <c r="AV4" s="24" t="s">
+      <c r="AO4" s="23"/>
+      <c r="AP4" s="23"/>
+      <c r="AQ4" s="23"/>
+      <c r="AR4" s="23"/>
+      <c r="AS4" s="23"/>
+      <c r="AT4" s="23"/>
+      <c r="AV4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="AW4" s="24"/>
-      <c r="AX4" s="24"/>
-      <c r="AY4" s="24"/>
-      <c r="AZ4" s="24"/>
-      <c r="BA4" s="24"/>
-      <c r="BB4" s="24" t="s">
+      <c r="AW4" s="23"/>
+      <c r="AX4" s="23"/>
+      <c r="AY4" s="23"/>
+      <c r="AZ4" s="23"/>
+      <c r="BA4" s="23"/>
+      <c r="BB4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="BC4" s="24"/>
-      <c r="BD4" s="24"/>
-      <c r="BE4" s="24"/>
-      <c r="BF4" s="24"/>
-      <c r="BG4" s="24"/>
-      <c r="BH4" s="24"/>
-      <c r="BJ4" s="24" t="s">
+      <c r="BC4" s="23"/>
+      <c r="BD4" s="23"/>
+      <c r="BE4" s="23"/>
+      <c r="BF4" s="23"/>
+      <c r="BG4" s="23"/>
+      <c r="BH4" s="23"/>
+      <c r="BJ4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="BK4" s="24"/>
-      <c r="BL4" s="24"/>
-      <c r="BM4" s="24"/>
-      <c r="BN4" s="24"/>
-      <c r="BO4" s="24"/>
-      <c r="BP4" s="24" t="s">
+      <c r="BK4" s="23"/>
+      <c r="BL4" s="23"/>
+      <c r="BM4" s="23"/>
+      <c r="BN4" s="23"/>
+      <c r="BO4" s="23"/>
+      <c r="BP4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="BQ4" s="24"/>
-      <c r="BR4" s="24"/>
-      <c r="BS4" s="24"/>
-      <c r="BT4" s="24"/>
-      <c r="BU4" s="24"/>
-      <c r="BV4" s="24"/>
-      <c r="BW4" s="24"/>
-      <c r="BY4" s="24" t="s">
+      <c r="BQ4" s="23"/>
+      <c r="BR4" s="23"/>
+      <c r="BS4" s="23"/>
+      <c r="BT4" s="23"/>
+      <c r="BU4" s="23"/>
+      <c r="BV4" s="23"/>
+      <c r="BW4" s="23"/>
+      <c r="BY4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="BZ4" s="24"/>
-      <c r="CA4" s="24"/>
-      <c r="CB4" s="24"/>
-      <c r="CC4" s="24"/>
-      <c r="CD4" s="24"/>
-      <c r="CE4" s="24" t="s">
+      <c r="BZ4" s="23"/>
+      <c r="CA4" s="23"/>
+      <c r="CB4" s="23"/>
+      <c r="CC4" s="23"/>
+      <c r="CD4" s="23"/>
+      <c r="CE4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="CF4" s="24"/>
-      <c r="CG4" s="24"/>
-      <c r="CH4" s="24"/>
-      <c r="CI4" s="24"/>
-      <c r="CJ4" s="24"/>
-      <c r="CK4" s="24"/>
-      <c r="CM4" s="24" t="s">
+      <c r="CF4" s="23"/>
+      <c r="CG4" s="23"/>
+      <c r="CH4" s="23"/>
+      <c r="CI4" s="23"/>
+      <c r="CJ4" s="23"/>
+      <c r="CK4" s="23"/>
+      <c r="CM4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="CN4" s="24"/>
-      <c r="CO4" s="24"/>
-      <c r="CP4" s="24"/>
-      <c r="CQ4" s="24"/>
-      <c r="CR4" s="24"/>
-      <c r="CS4" s="24" t="s">
+      <c r="CN4" s="23"/>
+      <c r="CO4" s="23"/>
+      <c r="CP4" s="23"/>
+      <c r="CQ4" s="23"/>
+      <c r="CR4" s="23"/>
+      <c r="CS4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="CT4" s="24"/>
-      <c r="CU4" s="24"/>
-      <c r="CV4" s="24"/>
-      <c r="CW4" s="24"/>
-      <c r="CX4" s="24"/>
-      <c r="CY4" s="24"/>
-      <c r="CZ4" s="24"/>
+      <c r="CT4" s="23"/>
+      <c r="CU4" s="23"/>
+      <c r="CV4" s="23"/>
+      <c r="CW4" s="23"/>
+      <c r="CX4" s="23"/>
+      <c r="CY4" s="23"/>
+      <c r="CZ4" s="23"/>
     </row>
-    <row r="5" ht="14">
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="22" t="s">
+    <row r="5" spans="2:106" ht="14.4">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24" t="s">
+      <c r="H5" s="23"/>
+      <c r="I5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25" t="s">
+      <c r="J5" s="23"/>
+      <c r="K5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24" t="s">
+      <c r="N5" s="23"/>
+      <c r="O5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="25" t="s">
+      <c r="P5" s="23"/>
+      <c r="Q5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="R5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24" t="s">
+      <c r="V5" s="23"/>
+      <c r="W5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="25" t="s">
+      <c r="X5" s="23"/>
+      <c r="Y5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="Z5" s="22" t="s">
+      <c r="Z5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AA5" s="24" t="s">
+      <c r="AA5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24" t="s">
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AD5" s="24"/>
-      <c r="AE5" s="25" t="s">
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AF5" s="25" t="s">
+      <c r="AF5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AH5" s="22" t="s">
+      <c r="AH5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AI5" s="24" t="s">
+      <c r="AI5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AJ5" s="24"/>
-      <c r="AK5" s="24" t="s">
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AL5" s="24"/>
-      <c r="AM5" s="25" t="s">
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AN5" s="22" t="s">
+      <c r="AN5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="AO5" s="24" t="s">
+      <c r="AO5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AP5" s="24"/>
-      <c r="AQ5" s="24" t="s">
+      <c r="AP5" s="23"/>
+      <c r="AQ5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AR5" s="24"/>
-      <c r="AS5" s="25" t="s">
+      <c r="AR5" s="23"/>
+      <c r="AS5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="AT5" s="25" t="s">
+      <c r="AT5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="AV5" s="22" t="s">
+      <c r="AV5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AW5" s="24" t="s">
+      <c r="AW5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="AX5" s="24"/>
-      <c r="AY5" s="24" t="s">
+      <c r="AX5" s="23"/>
+      <c r="AY5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="AZ5" s="24"/>
-      <c r="BA5" s="25" t="s">
+      <c r="AZ5" s="23"/>
+      <c r="BA5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BB5" s="22" t="s">
+      <c r="BB5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="BC5" s="24" t="s">
+      <c r="BC5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="BD5" s="24"/>
-      <c r="BE5" s="24" t="s">
+      <c r="BD5" s="23"/>
+      <c r="BE5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="BF5" s="24"/>
-      <c r="BG5" s="25" t="s">
+      <c r="BF5" s="23"/>
+      <c r="BG5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BH5" s="25" t="s">
+      <c r="BH5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="BJ5" s="22" t="s">
+      <c r="BJ5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="BK5" s="24" t="s">
+      <c r="BK5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="BL5" s="24"/>
-      <c r="BM5" s="24" t="s">
+      <c r="BL5" s="23"/>
+      <c r="BM5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="BN5" s="24"/>
-      <c r="BO5" s="25" t="s">
+      <c r="BN5" s="23"/>
+      <c r="BO5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BP5" s="22" t="s">
+      <c r="BP5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="BQ5" s="24" t="s">
+      <c r="BQ5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="BR5" s="24"/>
-      <c r="BS5" s="24" t="s">
+      <c r="BR5" s="23"/>
+      <c r="BS5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="BT5" s="24"/>
-      <c r="BU5" s="25" t="s">
+      <c r="BT5" s="23"/>
+      <c r="BU5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BV5" s="25" t="s">
+      <c r="BV5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="BW5" s="25" t="s">
+      <c r="BW5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="BY5" s="22" t="s">
+      <c r="BY5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="BZ5" s="24" t="s">
+      <c r="BZ5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="CA5" s="24"/>
-      <c r="CB5" s="24" t="s">
+      <c r="CA5" s="23"/>
+      <c r="CB5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="CC5" s="24"/>
-      <c r="CD5" s="25" t="s">
+      <c r="CC5" s="23"/>
+      <c r="CD5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="CE5" s="22" t="s">
+      <c r="CE5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="CF5" s="24" t="s">
+      <c r="CF5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="CG5" s="24"/>
-      <c r="CH5" s="24" t="s">
+      <c r="CG5" s="23"/>
+      <c r="CH5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="CI5" s="24"/>
-      <c r="CJ5" s="25" t="s">
+      <c r="CI5" s="23"/>
+      <c r="CJ5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="CK5" s="25" t="s">
+      <c r="CK5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="CM5" s="22" t="s">
+      <c r="CM5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="CN5" s="24" t="s">
+      <c r="CN5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="CO5" s="24"/>
-      <c r="CP5" s="24" t="s">
+      <c r="CO5" s="23"/>
+      <c r="CP5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="CQ5" s="24"/>
-      <c r="CR5" s="25" t="s">
+      <c r="CQ5" s="23"/>
+      <c r="CR5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="CS5" s="22" t="s">
+      <c r="CS5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="CT5" s="24" t="s">
+      <c r="CT5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="CU5" s="24"/>
-      <c r="CV5" s="24" t="s">
+      <c r="CU5" s="23"/>
+      <c r="CV5" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="CW5" s="24"/>
-      <c r="CX5" s="25" t="s">
+      <c r="CW5" s="23"/>
+      <c r="CX5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="CY5" s="25" t="s">
+      <c r="CY5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="CZ5" s="25" t="s">
+      <c r="CZ5" s="24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" ht="14">
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="22"/>
+    <row r="6" spans="2:106" ht="14.4">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1654,8 +1588,8 @@
       <c r="J6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
       <c r="M6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1668,9 +1602,9 @@
       <c r="P6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
-      <c r="T6" s="22"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="T6" s="21"/>
       <c r="U6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1683,8 +1617,8 @@
       <c r="X6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Y6" s="22"/>
-      <c r="Z6" s="22"/>
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
       <c r="AA6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1697,9 +1631,9 @@
       <c r="AD6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AE6" s="22"/>
-      <c r="AF6" s="22"/>
-      <c r="AH6" s="22"/>
+      <c r="AE6" s="21"/>
+      <c r="AF6" s="21"/>
+      <c r="AH6" s="21"/>
       <c r="AI6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1712,8 +1646,8 @@
       <c r="AL6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AM6" s="22"/>
-      <c r="AN6" s="22"/>
+      <c r="AM6" s="21"/>
+      <c r="AN6" s="21"/>
       <c r="AO6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1726,9 +1660,9 @@
       <c r="AR6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AS6" s="22"/>
-      <c r="AT6" s="22"/>
-      <c r="AV6" s="22"/>
+      <c r="AS6" s="21"/>
+      <c r="AT6" s="21"/>
+      <c r="AV6" s="21"/>
       <c r="AW6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1741,8 +1675,8 @@
       <c r="AZ6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="BA6" s="22"/>
-      <c r="BB6" s="22"/>
+      <c r="BA6" s="21"/>
+      <c r="BB6" s="21"/>
       <c r="BC6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1755,9 +1689,9 @@
       <c r="BF6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="BG6" s="22"/>
-      <c r="BH6" s="22"/>
-      <c r="BJ6" s="22"/>
+      <c r="BG6" s="21"/>
+      <c r="BH6" s="21"/>
+      <c r="BJ6" s="21"/>
       <c r="BK6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1770,8 +1704,8 @@
       <c r="BN6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="BO6" s="22"/>
-      <c r="BP6" s="22"/>
+      <c r="BO6" s="21"/>
+      <c r="BP6" s="21"/>
       <c r="BQ6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1784,10 +1718,10 @@
       <c r="BT6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="BU6" s="22"/>
-      <c r="BV6" s="22"/>
-      <c r="BW6" s="22"/>
-      <c r="BY6" s="22"/>
+      <c r="BU6" s="21"/>
+      <c r="BV6" s="21"/>
+      <c r="BW6" s="21"/>
+      <c r="BY6" s="21"/>
       <c r="BZ6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1800,8 +1734,8 @@
       <c r="CC6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="CD6" s="22"/>
-      <c r="CE6" s="22"/>
+      <c r="CD6" s="21"/>
+      <c r="CE6" s="21"/>
       <c r="CF6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1814,9 +1748,9 @@
       <c r="CI6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="CJ6" s="22"/>
-      <c r="CK6" s="22"/>
-      <c r="CM6" s="22"/>
+      <c r="CJ6" s="21"/>
+      <c r="CK6" s="21"/>
+      <c r="CM6" s="21"/>
       <c r="CN6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1829,8 +1763,8 @@
       <c r="CQ6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="CR6" s="22"/>
-      <c r="CS6" s="22"/>
+      <c r="CR6" s="21"/>
+      <c r="CS6" s="21"/>
       <c r="CT6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1843,11 +1777,11 @@
       <c r="CW6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="CX6" s="22"/>
-      <c r="CY6" s="22"/>
-      <c r="CZ6" s="22"/>
+      <c r="CX6" s="21"/>
+      <c r="CY6" s="21"/>
+      <c r="CZ6" s="21"/>
     </row>
-    <row r="7" customHeight="1" ht="18">
+    <row r="7" spans="2:106" ht="18" customHeight="1">
       <c r="B7" s="11">
         <v>1</v>
       </c>
@@ -1858,7 +1792,7 @@
         <v>29</v>
       </c>
       <c r="E7" s="14" t="str">
-        <f>'定数'!D5</f>
+        <f>定数!D5</f>
         <v>チーム1</v>
       </c>
       <c r="F7" s="14" t="s">
@@ -1900,15 +1834,15 @@
       </c>
       <c r="R7" s="17"/>
       <c r="T7" s="14" t="str">
-        <f>F7</f>
+        <f t="shared" ref="T7:T15" si="0">F7</f>
         <v>金原 優太</v>
       </c>
       <c r="U7" s="15">
-        <f>N7+1</f>
+        <f t="shared" ref="U7:U15" si="1">N7+1</f>
         <v>44812</v>
       </c>
       <c r="V7" s="15">
-        <f>U7</f>
+        <f t="shared" ref="V7:V15" si="2">U7</f>
         <v>44812</v>
       </c>
       <c r="W7" s="15">
@@ -1925,27 +1859,33 @@
         <v>陶丽丽</v>
       </c>
       <c r="AA7" s="15">
-        <f>V7+1</f>
+        <f t="shared" ref="AA7:AA15" si="3">V7+1</f>
         <v>44813</v>
       </c>
       <c r="AB7" s="15">
-        <f>AA7</f>
+        <f t="shared" ref="AB7:AB15" si="4">AA7</f>
         <v>44813</v>
       </c>
-      <c r="AC7" s="15"/>
-      <c r="AD7" s="15"/>
-      <c r="AE7" s="17"/>
+      <c r="AC7" s="15">
+        <v>44816</v>
+      </c>
+      <c r="AD7" s="15">
+        <v>44816</v>
+      </c>
+      <c r="AE7" s="17">
+        <v>1</v>
+      </c>
       <c r="AF7" s="17"/>
       <c r="AH7" s="14" t="str">
-        <f>T7</f>
+        <f t="shared" ref="AH7:AH15" si="5">T7</f>
         <v>金原 優太</v>
       </c>
       <c r="AI7" s="15">
-        <f>AB7+3</f>
+        <f t="shared" ref="AI7:AI15" si="6">AB7+3</f>
         <v>44816</v>
       </c>
       <c r="AJ7" s="15">
-        <f>AI7</f>
+        <f t="shared" ref="AJ7:AJ15" si="7">AI7</f>
         <v>44816</v>
       </c>
       <c r="AK7" s="15"/>
@@ -1956,11 +1896,11 @@
         <v>陶丽丽</v>
       </c>
       <c r="AO7" s="15">
-        <f>AJ7+1</f>
+        <f t="shared" ref="AO7:AO15" si="8">AJ7+1</f>
         <v>44817</v>
       </c>
       <c r="AP7" s="15">
-        <f>AO7</f>
+        <f t="shared" ref="AP7:AP15" si="9">AO7</f>
         <v>44817</v>
       </c>
       <c r="AQ7" s="15"/>
@@ -1968,15 +1908,15 @@
       <c r="AS7" s="17"/>
       <c r="AT7" s="17"/>
       <c r="AV7" s="14" t="str">
-        <f>AH7</f>
+        <f t="shared" ref="AV7:AV15" si="10">AH7</f>
         <v>金原 優太</v>
       </c>
       <c r="AW7" s="15">
-        <f>AP7+1</f>
+        <f t="shared" ref="AW7:AW15" si="11">AP7+1</f>
         <v>44818</v>
       </c>
       <c r="AX7" s="15">
-        <f>AW7</f>
+        <f t="shared" ref="AX7:AX15" si="12">AW7</f>
         <v>44818</v>
       </c>
       <c r="AY7" s="15"/>
@@ -1987,11 +1927,11 @@
         <v>陶丽丽</v>
       </c>
       <c r="BC7" s="15">
-        <f>AX7+1</f>
+        <f t="shared" ref="BC7:BC15" si="13">AX7+1</f>
         <v>44819</v>
       </c>
       <c r="BD7" s="15">
-        <f>BC7</f>
+        <f t="shared" ref="BD7:BD15" si="14">BC7</f>
         <v>44819</v>
       </c>
       <c r="BE7" s="15"/>
@@ -1999,15 +1939,15 @@
       <c r="BG7" s="17"/>
       <c r="BH7" s="17"/>
       <c r="BJ7" s="14" t="str">
-        <f>AV7</f>
+        <f t="shared" ref="BJ7:BJ15" si="15">AV7</f>
         <v>金原 優太</v>
       </c>
       <c r="BK7" s="15">
-        <f>BD7+1</f>
+        <f t="shared" ref="BK7:BK15" si="16">BD7+1</f>
         <v>44820</v>
       </c>
       <c r="BL7" s="15">
-        <f>BK7</f>
+        <f t="shared" ref="BL7:BL15" si="17">BK7</f>
         <v>44820</v>
       </c>
       <c r="BM7" s="15"/>
@@ -2018,11 +1958,11 @@
         <v>陶丽丽</v>
       </c>
       <c r="BQ7" s="15">
-        <f>BL7+4</f>
+        <f t="shared" ref="BQ7:BQ15" si="18">BL7+4</f>
         <v>44824</v>
       </c>
       <c r="BR7" s="15">
-        <f>BQ7</f>
+        <f t="shared" ref="BR7:BR15" si="19">BQ7</f>
         <v>44824</v>
       </c>
       <c r="BS7" s="15"/>
@@ -2032,83 +1972,83 @@
       <c r="BW7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="BY7" s="26" t="str">
+      <c r="BY7" s="25" t="str">
         <f>E7</f>
         <v>チーム1</v>
       </c>
-      <c r="BZ7" s="29">
+      <c r="BZ7" s="28">
         <f>BQ7+1</f>
         <v>44825</v>
       </c>
-      <c r="CA7" s="29">
+      <c r="CA7" s="28">
         <f>BZ7</f>
         <v>44825</v>
       </c>
-      <c r="CB7" s="29"/>
-      <c r="CC7" s="29"/>
-      <c r="CD7" s="32"/>
-      <c r="CE7" s="35" t="str">
+      <c r="CB7" s="28"/>
+      <c r="CC7" s="28"/>
+      <c r="CD7" s="31"/>
+      <c r="CE7" s="34" t="str">
         <f>BY10</f>
         <v>チーム2</v>
       </c>
-      <c r="CF7" s="36">
+      <c r="CF7" s="35">
         <f>CA7</f>
         <v>44825</v>
       </c>
-      <c r="CG7" s="36">
+      <c r="CG7" s="35">
         <f>CF7</f>
         <v>44825</v>
       </c>
-      <c r="CH7" s="36"/>
-      <c r="CI7" s="36"/>
-      <c r="CJ7" s="37"/>
-      <c r="CK7" s="32"/>
-      <c r="CM7" s="26" t="str">
+      <c r="CH7" s="35"/>
+      <c r="CI7" s="35"/>
+      <c r="CJ7" s="36"/>
+      <c r="CK7" s="31"/>
+      <c r="CM7" s="25" t="str">
         <f>BY7</f>
         <v>チーム1</v>
       </c>
-      <c r="CN7" s="29">
+      <c r="CN7" s="28">
         <f>CF7</f>
         <v>44825</v>
       </c>
-      <c r="CO7" s="29">
+      <c r="CO7" s="28">
         <f>CN7</f>
         <v>44825</v>
       </c>
-      <c r="CP7" s="29"/>
-      <c r="CQ7" s="29"/>
-      <c r="CR7" s="32"/>
-      <c r="CS7" s="35" t="str">
+      <c r="CP7" s="28"/>
+      <c r="CQ7" s="28"/>
+      <c r="CR7" s="31"/>
+      <c r="CS7" s="34" t="str">
         <f>CM7</f>
         <v>チーム1</v>
       </c>
-      <c r="CT7" s="36">
+      <c r="CT7" s="35">
         <f>CO7</f>
         <v>44825</v>
       </c>
-      <c r="CU7" s="36">
+      <c r="CU7" s="35">
         <f>CT7</f>
         <v>44825</v>
       </c>
-      <c r="CV7" s="36"/>
-      <c r="CW7" s="36"/>
-      <c r="CX7" s="37"/>
-      <c r="CY7" s="37"/>
-      <c r="CZ7" s="37"/>
+      <c r="CV7" s="35"/>
+      <c r="CW7" s="35"/>
+      <c r="CX7" s="36"/>
+      <c r="CY7" s="36"/>
+      <c r="CZ7" s="36"/>
       <c r="DB7" s="19"/>
     </row>
-    <row r="8" customHeight="1" ht="18">
+    <row r="8" spans="2:106" ht="18" customHeight="1">
       <c r="B8" s="11">
         <v>2</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="37" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="14" t="str">
-        <f>'定数'!D5</f>
+        <f>定数!D5</f>
         <v>チーム1</v>
       </c>
       <c r="F8" s="14" t="s">
@@ -2150,34 +2090,36 @@
       </c>
       <c r="R8" s="17"/>
       <c r="T8" s="14" t="str">
-        <f>F8</f>
+        <f t="shared" si="0"/>
         <v>陶丽丽</v>
       </c>
       <c r="U8" s="15">
-        <f>N8+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V8" s="15">
-        <f>U8</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W8" s="15">
         <v>44813</v>
       </c>
-      <c r="X8" s="15"/>
+      <c r="X8" s="15">
+        <v>44816</v>
+      </c>
       <c r="Y8" s="17">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="18" t="str">
         <f>T9</f>
         <v>武欣月</v>
       </c>
       <c r="AA8" s="15">
-        <f>V8+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB8" s="15">
-        <f>AA8</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC8" s="15"/>
@@ -2185,15 +2127,15 @@
       <c r="AE8" s="17"/>
       <c r="AF8" s="17"/>
       <c r="AH8" s="14" t="str">
-        <f>T8</f>
+        <f t="shared" si="5"/>
         <v>陶丽丽</v>
       </c>
       <c r="AI8" s="15">
-        <f>AB8+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ8" s="15">
-        <f>AI8</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK8" s="15"/>
@@ -2204,11 +2146,11 @@
         <v>武欣月</v>
       </c>
       <c r="AO8" s="15">
-        <f>AJ8+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP8" s="15">
-        <f>AO8</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ8" s="15"/>
@@ -2216,15 +2158,15 @@
       <c r="AS8" s="17"/>
       <c r="AT8" s="17"/>
       <c r="AV8" s="14" t="str">
-        <f>AH8</f>
+        <f t="shared" si="10"/>
         <v>陶丽丽</v>
       </c>
       <c r="AW8" s="15">
-        <f>AP8+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX8" s="15">
-        <f>AW8</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY8" s="15"/>
@@ -2235,11 +2177,11 @@
         <v>武欣月</v>
       </c>
       <c r="BC8" s="15">
-        <f>AX8+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD8" s="15">
-        <f>BC8</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE8" s="15"/>
@@ -2247,15 +2189,15 @@
       <c r="BG8" s="17"/>
       <c r="BH8" s="17"/>
       <c r="BJ8" s="14" t="str">
-        <f>AV8</f>
+        <f t="shared" si="15"/>
         <v>陶丽丽</v>
       </c>
       <c r="BK8" s="15">
-        <f>BD8+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL8" s="15">
-        <f>BK8</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM8" s="15"/>
@@ -2266,11 +2208,11 @@
         <v>武欣月</v>
       </c>
       <c r="BQ8" s="15">
-        <f>BL8+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR8" s="15">
-        <f>BQ8</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS8" s="15"/>
@@ -2278,44 +2220,44 @@
       <c r="BU8" s="17"/>
       <c r="BV8" s="17"/>
       <c r="BW8" s="17"/>
-      <c r="BY8" s="27"/>
-      <c r="BZ8" s="30"/>
-      <c r="CA8" s="30"/>
-      <c r="CB8" s="30"/>
-      <c r="CC8" s="30"/>
-      <c r="CD8" s="33"/>
-      <c r="CE8" s="35"/>
-      <c r="CF8" s="36"/>
-      <c r="CG8" s="36"/>
-      <c r="CH8" s="36"/>
-      <c r="CI8" s="36"/>
-      <c r="CJ8" s="37"/>
-      <c r="CK8" s="33"/>
-      <c r="CM8" s="27"/>
-      <c r="CN8" s="30"/>
-      <c r="CO8" s="30"/>
-      <c r="CP8" s="30"/>
-      <c r="CQ8" s="30"/>
-      <c r="CR8" s="33"/>
-      <c r="CS8" s="35"/>
-      <c r="CT8" s="36"/>
-      <c r="CU8" s="36"/>
-      <c r="CV8" s="36"/>
-      <c r="CW8" s="36"/>
-      <c r="CX8" s="37"/>
-      <c r="CY8" s="37"/>
-      <c r="CZ8" s="37"/>
+      <c r="BY8" s="26"/>
+      <c r="BZ8" s="29"/>
+      <c r="CA8" s="29"/>
+      <c r="CB8" s="29"/>
+      <c r="CC8" s="29"/>
+      <c r="CD8" s="32"/>
+      <c r="CE8" s="34"/>
+      <c r="CF8" s="35"/>
+      <c r="CG8" s="35"/>
+      <c r="CH8" s="35"/>
+      <c r="CI8" s="35"/>
+      <c r="CJ8" s="36"/>
+      <c r="CK8" s="32"/>
+      <c r="CM8" s="26"/>
+      <c r="CN8" s="29"/>
+      <c r="CO8" s="29"/>
+      <c r="CP8" s="29"/>
+      <c r="CQ8" s="29"/>
+      <c r="CR8" s="32"/>
+      <c r="CS8" s="34"/>
+      <c r="CT8" s="35"/>
+      <c r="CU8" s="35"/>
+      <c r="CV8" s="35"/>
+      <c r="CW8" s="35"/>
+      <c r="CX8" s="36"/>
+      <c r="CY8" s="36"/>
+      <c r="CZ8" s="36"/>
     </row>
-    <row r="9" customHeight="1" ht="18">
+    <row r="9" spans="2:106" ht="18" customHeight="1">
       <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="13" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="14" t="str">
-        <f>'定数'!D5</f>
+        <f>定数!D5</f>
         <v>チーム1</v>
       </c>
       <c r="F9" s="14" t="s">
@@ -2357,15 +2299,15 @@
       </c>
       <c r="R9" s="17"/>
       <c r="T9" s="14" t="str">
-        <f>F9</f>
+        <f t="shared" si="0"/>
         <v>武欣月</v>
       </c>
       <c r="U9" s="15">
-        <f>N9+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V9" s="15">
-        <f>U9</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W9" s="15"/>
@@ -2376,11 +2318,11 @@
         <v>金原 優太</v>
       </c>
       <c r="AA9" s="15">
-        <f>V9+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB9" s="15">
-        <f>AA9</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC9" s="15"/>
@@ -2388,15 +2330,15 @@
       <c r="AE9" s="17"/>
       <c r="AF9" s="17"/>
       <c r="AH9" s="14" t="str">
-        <f>T9</f>
+        <f t="shared" si="5"/>
         <v>武欣月</v>
       </c>
       <c r="AI9" s="15">
-        <f>AB9+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ9" s="15">
-        <f>AI9</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK9" s="15"/>
@@ -2407,11 +2349,11 @@
         <v>金原 優太</v>
       </c>
       <c r="AO9" s="15">
-        <f>AJ9+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP9" s="15">
-        <f>AO9</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ9" s="15"/>
@@ -2419,15 +2361,15 @@
       <c r="AS9" s="17"/>
       <c r="AT9" s="17"/>
       <c r="AV9" s="14" t="str">
-        <f>AH9</f>
+        <f t="shared" si="10"/>
         <v>武欣月</v>
       </c>
       <c r="AW9" s="15">
-        <f>AP9+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX9" s="15">
-        <f>AW9</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY9" s="15"/>
@@ -2438,11 +2380,11 @@
         <v>金原 優太</v>
       </c>
       <c r="BC9" s="15">
-        <f>AX9+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD9" s="15">
-        <f>BC9</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE9" s="15"/>
@@ -2450,15 +2392,15 @@
       <c r="BG9" s="17"/>
       <c r="BH9" s="17"/>
       <c r="BJ9" s="14" t="str">
-        <f>AV9</f>
+        <f t="shared" si="15"/>
         <v>武欣月</v>
       </c>
       <c r="BK9" s="15">
-        <f>BD9+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL9" s="15">
-        <f>BK9</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM9" s="15"/>
@@ -2469,11 +2411,11 @@
         <v>金原 優太</v>
       </c>
       <c r="BQ9" s="15">
-        <f>BL9+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR9" s="15">
-        <f>BQ9</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS9" s="15"/>
@@ -2481,46 +2423,46 @@
       <c r="BU9" s="17"/>
       <c r="BV9" s="17"/>
       <c r="BW9" s="17"/>
-      <c r="BY9" s="28"/>
-      <c r="BZ9" s="31"/>
-      <c r="CA9" s="31"/>
-      <c r="CB9" s="31"/>
-      <c r="CC9" s="31"/>
-      <c r="CD9" s="34"/>
-      <c r="CE9" s="35"/>
-      <c r="CF9" s="36"/>
-      <c r="CG9" s="36"/>
-      <c r="CH9" s="36"/>
-      <c r="CI9" s="36"/>
-      <c r="CJ9" s="37"/>
-      <c r="CK9" s="34"/>
-      <c r="CM9" s="28"/>
-      <c r="CN9" s="31"/>
-      <c r="CO9" s="31"/>
-      <c r="CP9" s="31"/>
-      <c r="CQ9" s="31"/>
-      <c r="CR9" s="34"/>
-      <c r="CS9" s="35"/>
-      <c r="CT9" s="36"/>
-      <c r="CU9" s="36"/>
-      <c r="CV9" s="36"/>
-      <c r="CW9" s="36"/>
-      <c r="CX9" s="37"/>
-      <c r="CY9" s="37"/>
-      <c r="CZ9" s="37"/>
+      <c r="BY9" s="27"/>
+      <c r="BZ9" s="30"/>
+      <c r="CA9" s="30"/>
+      <c r="CB9" s="30"/>
+      <c r="CC9" s="30"/>
+      <c r="CD9" s="33"/>
+      <c r="CE9" s="34"/>
+      <c r="CF9" s="35"/>
+      <c r="CG9" s="35"/>
+      <c r="CH9" s="35"/>
+      <c r="CI9" s="35"/>
+      <c r="CJ9" s="36"/>
+      <c r="CK9" s="33"/>
+      <c r="CM9" s="27"/>
+      <c r="CN9" s="30"/>
+      <c r="CO9" s="30"/>
+      <c r="CP9" s="30"/>
+      <c r="CQ9" s="30"/>
+      <c r="CR9" s="33"/>
+      <c r="CS9" s="34"/>
+      <c r="CT9" s="35"/>
+      <c r="CU9" s="35"/>
+      <c r="CV9" s="35"/>
+      <c r="CW9" s="35"/>
+      <c r="CX9" s="36"/>
+      <c r="CY9" s="36"/>
+      <c r="CZ9" s="36"/>
     </row>
-    <row r="10" customHeight="1" ht="18">
+    <row r="10" spans="2:106" ht="18" customHeight="1">
       <c r="B10" s="11">
         <v>4</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="37" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E10" s="14" t="str">
-        <f>'定数'!D8</f>
+        <f>定数!D8</f>
         <v>チーム2</v>
       </c>
       <c r="F10" s="14" t="s">
@@ -2556,15 +2498,15 @@
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
       <c r="T10" s="14" t="str">
-        <f>F10</f>
+        <f t="shared" si="0"/>
         <v>中山　裕司</v>
       </c>
       <c r="U10" s="15">
-        <f>N10+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V10" s="15">
-        <f>U10</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W10" s="15"/>
@@ -2575,11 +2517,11 @@
         <v>孫静孺</v>
       </c>
       <c r="AA10" s="15">
-        <f>V10+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB10" s="15">
-        <f>AA10</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC10" s="15"/>
@@ -2587,15 +2529,15 @@
       <c r="AE10" s="17"/>
       <c r="AF10" s="17"/>
       <c r="AH10" s="14" t="str">
-        <f>T10</f>
+        <f t="shared" si="5"/>
         <v>中山　裕司</v>
       </c>
       <c r="AI10" s="15">
-        <f>AB10+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ10" s="15">
-        <f>AI10</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK10" s="15"/>
@@ -2606,11 +2548,11 @@
         <v>孫静孺</v>
       </c>
       <c r="AO10" s="15">
-        <f>AJ10+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP10" s="15">
-        <f>AO10</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ10" s="15"/>
@@ -2618,15 +2560,15 @@
       <c r="AS10" s="17"/>
       <c r="AT10" s="17"/>
       <c r="AV10" s="14" t="str">
-        <f>AH10</f>
+        <f t="shared" si="10"/>
         <v>中山　裕司</v>
       </c>
       <c r="AW10" s="15">
-        <f>AP10+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX10" s="15">
-        <f>AW10</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY10" s="15"/>
@@ -2637,11 +2579,11 @@
         <v>孫静孺</v>
       </c>
       <c r="BC10" s="15">
-        <f>AX10+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD10" s="15">
-        <f>BC10</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE10" s="15"/>
@@ -2649,15 +2591,15 @@
       <c r="BG10" s="17"/>
       <c r="BH10" s="17"/>
       <c r="BJ10" s="14" t="str">
-        <f>AV10</f>
+        <f t="shared" si="15"/>
         <v>中山　裕司</v>
       </c>
       <c r="BK10" s="15">
-        <f>BD10+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL10" s="15">
-        <f>BK10</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM10" s="15"/>
@@ -2668,11 +2610,11 @@
         <v>孫静孺</v>
       </c>
       <c r="BQ10" s="15">
-        <f>BL10+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR10" s="15">
-        <f>BQ10</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS10" s="15"/>
@@ -2680,80 +2622,80 @@
       <c r="BU10" s="17"/>
       <c r="BV10" s="17"/>
       <c r="BW10" s="17"/>
-      <c r="BY10" s="26" t="str">
+      <c r="BY10" s="25" t="str">
         <f>E10</f>
         <v>チーム2</v>
       </c>
-      <c r="BZ10" s="29">
+      <c r="BZ10" s="28">
         <f>BQ10+1</f>
         <v>44825</v>
       </c>
-      <c r="CA10" s="29">
+      <c r="CA10" s="28">
         <f>BZ10</f>
         <v>44825</v>
       </c>
-      <c r="CB10" s="29"/>
-      <c r="CC10" s="29"/>
-      <c r="CD10" s="32"/>
-      <c r="CE10" s="35" t="str">
+      <c r="CB10" s="28"/>
+      <c r="CC10" s="28"/>
+      <c r="CD10" s="31"/>
+      <c r="CE10" s="34" t="str">
         <f>BY13</f>
         <v>チーム3</v>
       </c>
-      <c r="CF10" s="36">
+      <c r="CF10" s="35">
         <f>CA10</f>
         <v>44825</v>
       </c>
-      <c r="CG10" s="36">
+      <c r="CG10" s="35">
         <f>CF10</f>
         <v>44825</v>
       </c>
-      <c r="CH10" s="36"/>
-      <c r="CI10" s="36"/>
-      <c r="CJ10" s="37"/>
-      <c r="CK10" s="32"/>
-      <c r="CM10" s="26" t="str">
+      <c r="CH10" s="35"/>
+      <c r="CI10" s="35"/>
+      <c r="CJ10" s="36"/>
+      <c r="CK10" s="31"/>
+      <c r="CM10" s="25" t="str">
         <f>BY10</f>
         <v>チーム2</v>
       </c>
-      <c r="CN10" s="29">
+      <c r="CN10" s="28">
         <f>CF10</f>
         <v>44825</v>
       </c>
-      <c r="CO10" s="29">
+      <c r="CO10" s="28">
         <f>CN10</f>
         <v>44825</v>
       </c>
-      <c r="CP10" s="29"/>
-      <c r="CQ10" s="29"/>
-      <c r="CR10" s="32"/>
-      <c r="CS10" s="35" t="str">
+      <c r="CP10" s="28"/>
+      <c r="CQ10" s="28"/>
+      <c r="CR10" s="31"/>
+      <c r="CS10" s="34" t="str">
         <f>CM10</f>
         <v>チーム2</v>
       </c>
-      <c r="CT10" s="36">
+      <c r="CT10" s="35">
         <f>CO10</f>
         <v>44825</v>
       </c>
-      <c r="CU10" s="36">
+      <c r="CU10" s="35">
         <f>CT10</f>
         <v>44825</v>
       </c>
-      <c r="CV10" s="36"/>
-      <c r="CW10" s="36"/>
-      <c r="CX10" s="37"/>
-      <c r="CY10" s="37"/>
-      <c r="CZ10" s="37"/>
+      <c r="CV10" s="35"/>
+      <c r="CW10" s="35"/>
+      <c r="CX10" s="36"/>
+      <c r="CY10" s="36"/>
+      <c r="CZ10" s="36"/>
     </row>
-    <row r="11" customHeight="1" ht="18">
+    <row r="11" spans="2:106" ht="18" customHeight="1">
       <c r="B11" s="11">
         <v>5</v>
       </c>
-      <c r="C11" s="39"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="13" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="14" t="str">
-        <f>'定数'!D8</f>
+        <f>定数!D8</f>
         <v>チーム2</v>
       </c>
       <c r="F11" s="14" t="s">
@@ -2789,15 +2731,15 @@
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
       <c r="T11" s="14" t="str">
-        <f>F11</f>
+        <f t="shared" si="0"/>
         <v>孫静孺</v>
       </c>
       <c r="U11" s="15">
-        <f>N11+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V11" s="15">
-        <f>U11</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W11" s="15"/>
@@ -2808,11 +2750,11 @@
         <v>司徒健斌</v>
       </c>
       <c r="AA11" s="15">
-        <f>V11+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB11" s="15">
-        <f>AA11</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC11" s="15"/>
@@ -2820,15 +2762,15 @@
       <c r="AE11" s="17"/>
       <c r="AF11" s="17"/>
       <c r="AH11" s="14" t="str">
-        <f>T11</f>
+        <f t="shared" si="5"/>
         <v>孫静孺</v>
       </c>
       <c r="AI11" s="15">
-        <f>AB11+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ11" s="15">
-        <f>AI11</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK11" s="15"/>
@@ -2839,11 +2781,11 @@
         <v>司徒健斌</v>
       </c>
       <c r="AO11" s="15">
-        <f>AJ11+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP11" s="15">
-        <f>AO11</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ11" s="15"/>
@@ -2851,15 +2793,15 @@
       <c r="AS11" s="17"/>
       <c r="AT11" s="17"/>
       <c r="AV11" s="14" t="str">
-        <f>AH11</f>
+        <f t="shared" si="10"/>
         <v>孫静孺</v>
       </c>
       <c r="AW11" s="15">
-        <f>AP11+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX11" s="15">
-        <f>AW11</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY11" s="15"/>
@@ -2870,11 +2812,11 @@
         <v>司徒健斌</v>
       </c>
       <c r="BC11" s="15">
-        <f>AX11+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD11" s="15">
-        <f>BC11</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE11" s="15"/>
@@ -2882,15 +2824,15 @@
       <c r="BG11" s="17"/>
       <c r="BH11" s="17"/>
       <c r="BJ11" s="14" t="str">
-        <f>AV11</f>
+        <f t="shared" si="15"/>
         <v>孫静孺</v>
       </c>
       <c r="BK11" s="15">
-        <f>BD11+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL11" s="15">
-        <f>BK11</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM11" s="15"/>
@@ -2901,11 +2843,11 @@
         <v>司徒健斌</v>
       </c>
       <c r="BQ11" s="15">
-        <f>BL11+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR11" s="15">
-        <f>BQ11</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS11" s="15"/>
@@ -2913,44 +2855,44 @@
       <c r="BU11" s="17"/>
       <c r="BV11" s="17"/>
       <c r="BW11" s="17"/>
-      <c r="BY11" s="27"/>
-      <c r="BZ11" s="30"/>
-      <c r="CA11" s="30"/>
-      <c r="CB11" s="30"/>
-      <c r="CC11" s="30"/>
-      <c r="CD11" s="33"/>
-      <c r="CE11" s="35"/>
-      <c r="CF11" s="36"/>
-      <c r="CG11" s="36"/>
-      <c r="CH11" s="36"/>
-      <c r="CI11" s="36"/>
-      <c r="CJ11" s="37"/>
-      <c r="CK11" s="33"/>
-      <c r="CM11" s="27"/>
-      <c r="CN11" s="30"/>
-      <c r="CO11" s="30"/>
-      <c r="CP11" s="30"/>
-      <c r="CQ11" s="30"/>
-      <c r="CR11" s="33"/>
-      <c r="CS11" s="35"/>
-      <c r="CT11" s="36"/>
-      <c r="CU11" s="36"/>
-      <c r="CV11" s="36"/>
-      <c r="CW11" s="36"/>
-      <c r="CX11" s="37"/>
-      <c r="CY11" s="37"/>
-      <c r="CZ11" s="37"/>
+      <c r="BY11" s="26"/>
+      <c r="BZ11" s="29"/>
+      <c r="CA11" s="29"/>
+      <c r="CB11" s="29"/>
+      <c r="CC11" s="29"/>
+      <c r="CD11" s="32"/>
+      <c r="CE11" s="34"/>
+      <c r="CF11" s="35"/>
+      <c r="CG11" s="35"/>
+      <c r="CH11" s="35"/>
+      <c r="CI11" s="35"/>
+      <c r="CJ11" s="36"/>
+      <c r="CK11" s="32"/>
+      <c r="CM11" s="26"/>
+      <c r="CN11" s="29"/>
+      <c r="CO11" s="29"/>
+      <c r="CP11" s="29"/>
+      <c r="CQ11" s="29"/>
+      <c r="CR11" s="32"/>
+      <c r="CS11" s="34"/>
+      <c r="CT11" s="35"/>
+      <c r="CU11" s="35"/>
+      <c r="CV11" s="35"/>
+      <c r="CW11" s="35"/>
+      <c r="CX11" s="36"/>
+      <c r="CY11" s="36"/>
+      <c r="CZ11" s="36"/>
     </row>
-    <row r="12" customHeight="1" ht="18">
+    <row r="12" spans="2:106" ht="18" customHeight="1">
       <c r="B12" s="11">
         <v>6</v>
       </c>
-      <c r="C12" s="39"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E12" s="14" t="str">
-        <f>'定数'!D8</f>
+        <f>定数!D8</f>
         <v>チーム2</v>
       </c>
       <c r="F12" s="14" t="s">
@@ -2986,15 +2928,15 @@
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
       <c r="T12" s="14" t="str">
-        <f>F12</f>
+        <f t="shared" si="0"/>
         <v>司徒健斌</v>
       </c>
       <c r="U12" s="15">
-        <f>N12+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V12" s="15">
-        <f>U12</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W12" s="15"/>
@@ -3005,11 +2947,11 @@
         <v>中山　裕司</v>
       </c>
       <c r="AA12" s="15">
-        <f>V12+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB12" s="15">
-        <f>AA12</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC12" s="15"/>
@@ -3017,15 +2959,15 @@
       <c r="AE12" s="17"/>
       <c r="AF12" s="17"/>
       <c r="AH12" s="14" t="str">
-        <f>T12</f>
+        <f t="shared" si="5"/>
         <v>司徒健斌</v>
       </c>
       <c r="AI12" s="15">
-        <f>AB12+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ12" s="15">
-        <f>AI12</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK12" s="15"/>
@@ -3036,11 +2978,11 @@
         <v>中山　裕司</v>
       </c>
       <c r="AO12" s="15">
-        <f>AJ12+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP12" s="15">
-        <f>AO12</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ12" s="15"/>
@@ -3048,15 +2990,15 @@
       <c r="AS12" s="17"/>
       <c r="AT12" s="17"/>
       <c r="AV12" s="14" t="str">
-        <f>AH12</f>
+        <f t="shared" si="10"/>
         <v>司徒健斌</v>
       </c>
       <c r="AW12" s="15">
-        <f>AP12+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX12" s="15">
-        <f>AW12</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY12" s="15"/>
@@ -3067,11 +3009,11 @@
         <v>中山　裕司</v>
       </c>
       <c r="BC12" s="15">
-        <f>AX12+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD12" s="15">
-        <f>BC12</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE12" s="15"/>
@@ -3079,15 +3021,15 @@
       <c r="BG12" s="17"/>
       <c r="BH12" s="17"/>
       <c r="BJ12" s="14" t="str">
-        <f>AV12</f>
+        <f t="shared" si="15"/>
         <v>司徒健斌</v>
       </c>
       <c r="BK12" s="15">
-        <f>BD12+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL12" s="15">
-        <f>BK12</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM12" s="15"/>
@@ -3098,11 +3040,11 @@
         <v>中山　裕司</v>
       </c>
       <c r="BQ12" s="15">
-        <f>BL12+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR12" s="15">
-        <f>BQ12</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS12" s="15"/>
@@ -3110,46 +3052,46 @@
       <c r="BU12" s="17"/>
       <c r="BV12" s="17"/>
       <c r="BW12" s="17"/>
-      <c r="BY12" s="28"/>
-      <c r="BZ12" s="31"/>
-      <c r="CA12" s="31"/>
-      <c r="CB12" s="31"/>
-      <c r="CC12" s="31"/>
-      <c r="CD12" s="34"/>
-      <c r="CE12" s="35"/>
-      <c r="CF12" s="36"/>
-      <c r="CG12" s="36"/>
-      <c r="CH12" s="36"/>
-      <c r="CI12" s="36"/>
-      <c r="CJ12" s="37"/>
-      <c r="CK12" s="34"/>
-      <c r="CM12" s="28"/>
-      <c r="CN12" s="31"/>
-      <c r="CO12" s="31"/>
-      <c r="CP12" s="31"/>
-      <c r="CQ12" s="31"/>
-      <c r="CR12" s="34"/>
-      <c r="CS12" s="35"/>
-      <c r="CT12" s="36"/>
-      <c r="CU12" s="36"/>
-      <c r="CV12" s="36"/>
-      <c r="CW12" s="36"/>
-      <c r="CX12" s="37"/>
-      <c r="CY12" s="37"/>
-      <c r="CZ12" s="37"/>
+      <c r="BY12" s="27"/>
+      <c r="BZ12" s="30"/>
+      <c r="CA12" s="30"/>
+      <c r="CB12" s="30"/>
+      <c r="CC12" s="30"/>
+      <c r="CD12" s="33"/>
+      <c r="CE12" s="34"/>
+      <c r="CF12" s="35"/>
+      <c r="CG12" s="35"/>
+      <c r="CH12" s="35"/>
+      <c r="CI12" s="35"/>
+      <c r="CJ12" s="36"/>
+      <c r="CK12" s="33"/>
+      <c r="CM12" s="27"/>
+      <c r="CN12" s="30"/>
+      <c r="CO12" s="30"/>
+      <c r="CP12" s="30"/>
+      <c r="CQ12" s="30"/>
+      <c r="CR12" s="33"/>
+      <c r="CS12" s="34"/>
+      <c r="CT12" s="35"/>
+      <c r="CU12" s="35"/>
+      <c r="CV12" s="35"/>
+      <c r="CW12" s="35"/>
+      <c r="CX12" s="36"/>
+      <c r="CY12" s="36"/>
+      <c r="CZ12" s="36"/>
     </row>
-    <row r="13" customHeight="1" ht="18">
+    <row r="13" spans="2:106" ht="18" customHeight="1">
       <c r="B13" s="11">
         <v>7</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="39" t="s">
         <v>43</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="14" t="str">
-        <f>'定数'!D11</f>
+        <f>定数!D11</f>
         <v>チーム3</v>
       </c>
       <c r="F13" s="16" t="s">
@@ -3185,15 +3127,15 @@
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
       <c r="T13" s="14" t="str">
-        <f>F13</f>
+        <f t="shared" si="0"/>
         <v>张晓</v>
       </c>
       <c r="U13" s="15">
-        <f>N13+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V13" s="15">
-        <f>U13</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W13" s="15"/>
@@ -3204,11 +3146,11 @@
         <v>白宝帥</v>
       </c>
       <c r="AA13" s="15">
-        <f>V13+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB13" s="15">
-        <f>AA13</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC13" s="15"/>
@@ -3216,15 +3158,15 @@
       <c r="AE13" s="17"/>
       <c r="AF13" s="17"/>
       <c r="AH13" s="14" t="str">
-        <f>T13</f>
+        <f t="shared" si="5"/>
         <v>张晓</v>
       </c>
       <c r="AI13" s="15">
-        <f>AB13+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ13" s="15">
-        <f>AI13</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK13" s="15"/>
@@ -3235,11 +3177,11 @@
         <v>白宝帥</v>
       </c>
       <c r="AO13" s="15">
-        <f>AJ13+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP13" s="15">
-        <f>AO13</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ13" s="15"/>
@@ -3247,15 +3189,15 @@
       <c r="AS13" s="17"/>
       <c r="AT13" s="17"/>
       <c r="AV13" s="14" t="str">
-        <f>AH13</f>
+        <f t="shared" si="10"/>
         <v>张晓</v>
       </c>
       <c r="AW13" s="15">
-        <f>AP13+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX13" s="15">
-        <f>AW13</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY13" s="15"/>
@@ -3266,11 +3208,11 @@
         <v>白宝帥</v>
       </c>
       <c r="BC13" s="15">
-        <f>AX13+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD13" s="15">
-        <f>BC13</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE13" s="15"/>
@@ -3278,15 +3220,15 @@
       <c r="BG13" s="17"/>
       <c r="BH13" s="17"/>
       <c r="BJ13" s="14" t="str">
-        <f>AV13</f>
+        <f t="shared" si="15"/>
         <v>张晓</v>
       </c>
       <c r="BK13" s="15">
-        <f>BD13+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL13" s="15">
-        <f>BK13</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM13" s="15"/>
@@ -3297,11 +3239,11 @@
         <v>白宝帥</v>
       </c>
       <c r="BQ13" s="15">
-        <f>BL13+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR13" s="15">
-        <f>BQ13</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS13" s="15"/>
@@ -3309,80 +3251,80 @@
       <c r="BU13" s="17"/>
       <c r="BV13" s="17"/>
       <c r="BW13" s="17"/>
-      <c r="BY13" s="26" t="str">
+      <c r="BY13" s="25" t="str">
         <f>E13</f>
         <v>チーム3</v>
       </c>
-      <c r="BZ13" s="29">
+      <c r="BZ13" s="28">
         <f>BQ13+1</f>
         <v>44825</v>
       </c>
-      <c r="CA13" s="29">
+      <c r="CA13" s="28">
         <f>BZ13</f>
         <v>44825</v>
       </c>
-      <c r="CB13" s="29"/>
-      <c r="CC13" s="29"/>
-      <c r="CD13" s="32"/>
-      <c r="CE13" s="35" t="str">
+      <c r="CB13" s="28"/>
+      <c r="CC13" s="28"/>
+      <c r="CD13" s="31"/>
+      <c r="CE13" s="34" t="str">
         <f>BY7</f>
         <v>チーム1</v>
       </c>
-      <c r="CF13" s="36">
+      <c r="CF13" s="35">
         <f>CA13</f>
         <v>44825</v>
       </c>
-      <c r="CG13" s="36">
+      <c r="CG13" s="35">
         <f>CF13</f>
         <v>44825</v>
       </c>
-      <c r="CH13" s="36"/>
-      <c r="CI13" s="36"/>
-      <c r="CJ13" s="37"/>
-      <c r="CK13" s="32"/>
-      <c r="CM13" s="26" t="str">
+      <c r="CH13" s="35"/>
+      <c r="CI13" s="35"/>
+      <c r="CJ13" s="36"/>
+      <c r="CK13" s="31"/>
+      <c r="CM13" s="25" t="str">
         <f>BY13</f>
         <v>チーム3</v>
       </c>
-      <c r="CN13" s="29">
+      <c r="CN13" s="28">
         <f>CF13</f>
         <v>44825</v>
       </c>
-      <c r="CO13" s="29">
+      <c r="CO13" s="28">
         <f>CN13</f>
         <v>44825</v>
       </c>
-      <c r="CP13" s="29"/>
-      <c r="CQ13" s="29"/>
-      <c r="CR13" s="32"/>
-      <c r="CS13" s="35" t="str">
+      <c r="CP13" s="28"/>
+      <c r="CQ13" s="28"/>
+      <c r="CR13" s="31"/>
+      <c r="CS13" s="34" t="str">
         <f>CM13</f>
         <v>チーム3</v>
       </c>
-      <c r="CT13" s="36">
+      <c r="CT13" s="35">
         <f>CO13</f>
         <v>44825</v>
       </c>
-      <c r="CU13" s="36">
+      <c r="CU13" s="35">
         <f>CT13</f>
         <v>44825</v>
       </c>
-      <c r="CV13" s="36"/>
-      <c r="CW13" s="36"/>
-      <c r="CX13" s="37"/>
-      <c r="CY13" s="37"/>
-      <c r="CZ13" s="37"/>
+      <c r="CV13" s="35"/>
+      <c r="CW13" s="35"/>
+      <c r="CX13" s="36"/>
+      <c r="CY13" s="36"/>
+      <c r="CZ13" s="36"/>
     </row>
-    <row r="14" customHeight="1" ht="18">
+    <row r="14" spans="2:106" ht="18" customHeight="1">
       <c r="B14" s="11">
         <v>8</v>
       </c>
-      <c r="C14" s="39"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="13" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="14" t="str">
-        <f>'定数'!D11</f>
+        <f>定数!D11</f>
         <v>チーム3</v>
       </c>
       <c r="F14" s="14" t="s">
@@ -3418,15 +3360,15 @@
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
       <c r="T14" s="14" t="str">
-        <f>F14</f>
+        <f t="shared" si="0"/>
         <v>白宝帥</v>
       </c>
       <c r="U14" s="15">
-        <f>N14+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V14" s="15">
-        <f>U14</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W14" s="15"/>
@@ -3437,11 +3379,11 @@
         <v>趙小萱</v>
       </c>
       <c r="AA14" s="15">
-        <f>V14+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB14" s="15">
-        <f>AA14</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC14" s="15"/>
@@ -3449,15 +3391,15 @@
       <c r="AE14" s="17"/>
       <c r="AF14" s="17"/>
       <c r="AH14" s="14" t="str">
-        <f>T14</f>
+        <f t="shared" si="5"/>
         <v>白宝帥</v>
       </c>
       <c r="AI14" s="15">
-        <f>AB14+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ14" s="15">
-        <f>AI14</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK14" s="15"/>
@@ -3468,11 +3410,11 @@
         <v>趙小萱</v>
       </c>
       <c r="AO14" s="15">
-        <f>AJ14+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP14" s="15">
-        <f>AO14</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ14" s="15"/>
@@ -3480,15 +3422,15 @@
       <c r="AS14" s="17"/>
       <c r="AT14" s="17"/>
       <c r="AV14" s="14" t="str">
-        <f>AH14</f>
+        <f t="shared" si="10"/>
         <v>白宝帥</v>
       </c>
       <c r="AW14" s="15">
-        <f>AP14+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX14" s="15">
-        <f>AW14</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY14" s="15"/>
@@ -3499,11 +3441,11 @@
         <v>趙小萱</v>
       </c>
       <c r="BC14" s="15">
-        <f>AX14+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD14" s="15">
-        <f>BC14</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE14" s="15"/>
@@ -3511,15 +3453,15 @@
       <c r="BG14" s="17"/>
       <c r="BH14" s="17"/>
       <c r="BJ14" s="14" t="str">
-        <f>AV14</f>
+        <f t="shared" si="15"/>
         <v>白宝帥</v>
       </c>
       <c r="BK14" s="15">
-        <f>BD14+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL14" s="15">
-        <f>BK14</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM14" s="15"/>
@@ -3530,11 +3472,11 @@
         <v>趙小萱</v>
       </c>
       <c r="BQ14" s="15">
-        <f>BL14+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR14" s="15">
-        <f>BQ14</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS14" s="15"/>
@@ -3542,44 +3484,44 @@
       <c r="BU14" s="17"/>
       <c r="BV14" s="17"/>
       <c r="BW14" s="17"/>
-      <c r="BY14" s="27"/>
-      <c r="BZ14" s="30"/>
-      <c r="CA14" s="30"/>
-      <c r="CB14" s="30"/>
-      <c r="CC14" s="30"/>
-      <c r="CD14" s="33"/>
-      <c r="CE14" s="35"/>
-      <c r="CF14" s="36"/>
-      <c r="CG14" s="36"/>
-      <c r="CH14" s="36"/>
-      <c r="CI14" s="36"/>
-      <c r="CJ14" s="37"/>
-      <c r="CK14" s="33"/>
-      <c r="CM14" s="27"/>
-      <c r="CN14" s="30"/>
-      <c r="CO14" s="30"/>
-      <c r="CP14" s="30"/>
-      <c r="CQ14" s="30"/>
-      <c r="CR14" s="33"/>
-      <c r="CS14" s="35"/>
-      <c r="CT14" s="36"/>
-      <c r="CU14" s="36"/>
-      <c r="CV14" s="36"/>
-      <c r="CW14" s="36"/>
-      <c r="CX14" s="37"/>
-      <c r="CY14" s="37"/>
-      <c r="CZ14" s="37"/>
+      <c r="BY14" s="26"/>
+      <c r="BZ14" s="29"/>
+      <c r="CA14" s="29"/>
+      <c r="CB14" s="29"/>
+      <c r="CC14" s="29"/>
+      <c r="CD14" s="32"/>
+      <c r="CE14" s="34"/>
+      <c r="CF14" s="35"/>
+      <c r="CG14" s="35"/>
+      <c r="CH14" s="35"/>
+      <c r="CI14" s="35"/>
+      <c r="CJ14" s="36"/>
+      <c r="CK14" s="32"/>
+      <c r="CM14" s="26"/>
+      <c r="CN14" s="29"/>
+      <c r="CO14" s="29"/>
+      <c r="CP14" s="29"/>
+      <c r="CQ14" s="29"/>
+      <c r="CR14" s="32"/>
+      <c r="CS14" s="34"/>
+      <c r="CT14" s="35"/>
+      <c r="CU14" s="35"/>
+      <c r="CV14" s="35"/>
+      <c r="CW14" s="35"/>
+      <c r="CX14" s="36"/>
+      <c r="CY14" s="36"/>
+      <c r="CZ14" s="36"/>
     </row>
-    <row r="15" customHeight="1" ht="18">
+    <row r="15" spans="2:106" ht="18" customHeight="1">
       <c r="B15" s="11">
         <v>9</v>
       </c>
-      <c r="C15" s="39"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="14" t="str">
-        <f>'定数'!D11</f>
+        <f>定数!D11</f>
         <v>チーム3</v>
       </c>
       <c r="F15" s="14" t="s">
@@ -3609,15 +3551,15 @@
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
       <c r="T15" s="14" t="str">
-        <f>F15</f>
+        <f t="shared" si="0"/>
         <v>趙小萱</v>
       </c>
       <c r="U15" s="15">
-        <f>N15+1</f>
+        <f t="shared" si="1"/>
         <v>44812</v>
       </c>
       <c r="V15" s="15">
-        <f>U15</f>
+        <f t="shared" si="2"/>
         <v>44812</v>
       </c>
       <c r="W15" s="15"/>
@@ -3628,11 +3570,11 @@
         <v>张晓</v>
       </c>
       <c r="AA15" s="15">
-        <f>V15+1</f>
+        <f t="shared" si="3"/>
         <v>44813</v>
       </c>
       <c r="AB15" s="15">
-        <f>AA15</f>
+        <f t="shared" si="4"/>
         <v>44813</v>
       </c>
       <c r="AC15" s="15"/>
@@ -3640,15 +3582,15 @@
       <c r="AE15" s="17"/>
       <c r="AF15" s="17"/>
       <c r="AH15" s="14" t="str">
-        <f>T15</f>
+        <f t="shared" si="5"/>
         <v>趙小萱</v>
       </c>
       <c r="AI15" s="15">
-        <f>AB15+3</f>
+        <f t="shared" si="6"/>
         <v>44816</v>
       </c>
       <c r="AJ15" s="15">
-        <f>AI15</f>
+        <f t="shared" si="7"/>
         <v>44816</v>
       </c>
       <c r="AK15" s="15"/>
@@ -3659,11 +3601,11 @@
         <v>张晓</v>
       </c>
       <c r="AO15" s="15">
-        <f>AJ15+1</f>
+        <f t="shared" si="8"/>
         <v>44817</v>
       </c>
       <c r="AP15" s="15">
-        <f>AO15</f>
+        <f t="shared" si="9"/>
         <v>44817</v>
       </c>
       <c r="AQ15" s="15"/>
@@ -3671,15 +3613,15 @@
       <c r="AS15" s="17"/>
       <c r="AT15" s="17"/>
       <c r="AV15" s="14" t="str">
-        <f>AH15</f>
+        <f t="shared" si="10"/>
         <v>趙小萱</v>
       </c>
       <c r="AW15" s="15">
-        <f>AP15+1</f>
+        <f t="shared" si="11"/>
         <v>44818</v>
       </c>
       <c r="AX15" s="15">
-        <f>AW15</f>
+        <f t="shared" si="12"/>
         <v>44818</v>
       </c>
       <c r="AY15" s="15"/>
@@ -3690,11 +3632,11 @@
         <v>张晓</v>
       </c>
       <c r="BC15" s="15">
-        <f>AX15+1</f>
+        <f t="shared" si="13"/>
         <v>44819</v>
       </c>
       <c r="BD15" s="15">
-        <f>BC15</f>
+        <f t="shared" si="14"/>
         <v>44819</v>
       </c>
       <c r="BE15" s="15"/>
@@ -3702,15 +3644,15 @@
       <c r="BG15" s="17"/>
       <c r="BH15" s="17"/>
       <c r="BJ15" s="14" t="str">
-        <f>AV15</f>
+        <f t="shared" si="15"/>
         <v>趙小萱</v>
       </c>
       <c r="BK15" s="15">
-        <f>BD15+1</f>
+        <f t="shared" si="16"/>
         <v>44820</v>
       </c>
       <c r="BL15" s="15">
-        <f>BK15</f>
+        <f t="shared" si="17"/>
         <v>44820</v>
       </c>
       <c r="BM15" s="15"/>
@@ -3721,11 +3663,11 @@
         <v>张晓</v>
       </c>
       <c r="BQ15" s="15">
-        <f>BL15+4</f>
+        <f t="shared" si="18"/>
         <v>44824</v>
       </c>
       <c r="BR15" s="15">
-        <f>BQ15</f>
+        <f t="shared" si="19"/>
         <v>44824</v>
       </c>
       <c r="BS15" s="15"/>
@@ -3733,114 +3675,101 @@
       <c r="BU15" s="17"/>
       <c r="BV15" s="17"/>
       <c r="BW15" s="17"/>
-      <c r="BY15" s="28"/>
-      <c r="BZ15" s="31"/>
-      <c r="CA15" s="31"/>
-      <c r="CB15" s="31"/>
-      <c r="CC15" s="31"/>
-      <c r="CD15" s="34"/>
-      <c r="CE15" s="35"/>
-      <c r="CF15" s="36"/>
-      <c r="CG15" s="36"/>
-      <c r="CH15" s="36"/>
-      <c r="CI15" s="36"/>
-      <c r="CJ15" s="37"/>
-      <c r="CK15" s="34"/>
-      <c r="CM15" s="28"/>
-      <c r="CN15" s="31"/>
-      <c r="CO15" s="31"/>
-      <c r="CP15" s="31"/>
-      <c r="CQ15" s="31"/>
-      <c r="CR15" s="34"/>
-      <c r="CS15" s="35"/>
-      <c r="CT15" s="36"/>
-      <c r="CU15" s="36"/>
-      <c r="CV15" s="36"/>
-      <c r="CW15" s="36"/>
-      <c r="CX15" s="37"/>
-      <c r="CY15" s="37"/>
-      <c r="CZ15" s="37"/>
+      <c r="BY15" s="27"/>
+      <c r="BZ15" s="30"/>
+      <c r="CA15" s="30"/>
+      <c r="CB15" s="30"/>
+      <c r="CC15" s="30"/>
+      <c r="CD15" s="33"/>
+      <c r="CE15" s="34"/>
+      <c r="CF15" s="35"/>
+      <c r="CG15" s="35"/>
+      <c r="CH15" s="35"/>
+      <c r="CI15" s="35"/>
+      <c r="CJ15" s="36"/>
+      <c r="CK15" s="33"/>
+      <c r="CM15" s="27"/>
+      <c r="CN15" s="30"/>
+      <c r="CO15" s="30"/>
+      <c r="CP15" s="30"/>
+      <c r="CQ15" s="30"/>
+      <c r="CR15" s="33"/>
+      <c r="CS15" s="34"/>
+      <c r="CT15" s="35"/>
+      <c r="CU15" s="35"/>
+      <c r="CV15" s="35"/>
+      <c r="CW15" s="35"/>
+      <c r="CX15" s="36"/>
+      <c r="CY15" s="36"/>
+      <c r="CZ15" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="167">
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="T4:Y4"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="AH4:AM4"/>
-    <mergeCell ref="AN4:AT4"/>
-    <mergeCell ref="AV4:BA4"/>
-    <mergeCell ref="BB4:BH4"/>
-    <mergeCell ref="BJ4:BO4"/>
-    <mergeCell ref="BP4:BW4"/>
-    <mergeCell ref="BY4:CD4"/>
-    <mergeCell ref="CE4:CK4"/>
-    <mergeCell ref="CM4:CR4"/>
-    <mergeCell ref="CS4:CZ4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="T5:T6"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AE5:AE6"/>
-    <mergeCell ref="AF5:AF6"/>
-    <mergeCell ref="AH5:AH6"/>
-    <mergeCell ref="AI5:AJ5"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AM5:AM6"/>
-    <mergeCell ref="AN5:AN6"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AS5:AS6"/>
-    <mergeCell ref="AT5:AT6"/>
-    <mergeCell ref="AV5:AV6"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="BA5:BA6"/>
-    <mergeCell ref="BB5:BB6"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BH5:BH6"/>
-    <mergeCell ref="BJ5:BJ6"/>
-    <mergeCell ref="BK5:BL5"/>
-    <mergeCell ref="BM5:BN5"/>
-    <mergeCell ref="BO5:BO6"/>
-    <mergeCell ref="BP5:BP6"/>
-    <mergeCell ref="BQ5:BR5"/>
-    <mergeCell ref="BS5:BT5"/>
-    <mergeCell ref="BU5:BU6"/>
-    <mergeCell ref="BV5:BV6"/>
-    <mergeCell ref="BW5:BW6"/>
-    <mergeCell ref="BY5:BY6"/>
-    <mergeCell ref="BZ5:CA5"/>
-    <mergeCell ref="CB5:CC5"/>
-    <mergeCell ref="CD5:CD6"/>
-    <mergeCell ref="CE5:CE6"/>
-    <mergeCell ref="CF5:CG5"/>
-    <mergeCell ref="CH5:CI5"/>
-    <mergeCell ref="CJ5:CJ6"/>
-    <mergeCell ref="CK5:CK6"/>
-    <mergeCell ref="CM5:CM6"/>
-    <mergeCell ref="CN5:CO5"/>
-    <mergeCell ref="CP5:CQ5"/>
-    <mergeCell ref="CR5:CR6"/>
-    <mergeCell ref="CS5:CS6"/>
+    <mergeCell ref="CV13:CV15"/>
+    <mergeCell ref="CW13:CW15"/>
+    <mergeCell ref="CX13:CX15"/>
+    <mergeCell ref="CY13:CY15"/>
+    <mergeCell ref="CZ13:CZ15"/>
+    <mergeCell ref="CZ10:CZ12"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="BY13:BY15"/>
+    <mergeCell ref="BZ13:BZ15"/>
+    <mergeCell ref="CA13:CA15"/>
+    <mergeCell ref="CB13:CB15"/>
+    <mergeCell ref="CC13:CC15"/>
+    <mergeCell ref="CD13:CD15"/>
+    <mergeCell ref="CE13:CE15"/>
+    <mergeCell ref="CF13:CF15"/>
+    <mergeCell ref="CG13:CG15"/>
+    <mergeCell ref="CH13:CH15"/>
+    <mergeCell ref="CI13:CI15"/>
+    <mergeCell ref="CJ13:CJ15"/>
+    <mergeCell ref="CK13:CK15"/>
+    <mergeCell ref="CM13:CM15"/>
+    <mergeCell ref="CN13:CN15"/>
+    <mergeCell ref="CO13:CO15"/>
+    <mergeCell ref="CP13:CP15"/>
+    <mergeCell ref="CQ13:CQ15"/>
+    <mergeCell ref="CR13:CR15"/>
+    <mergeCell ref="CS13:CS15"/>
+    <mergeCell ref="CT13:CT15"/>
+    <mergeCell ref="CU13:CU15"/>
+    <mergeCell ref="CQ10:CQ12"/>
+    <mergeCell ref="CR10:CR12"/>
+    <mergeCell ref="CS10:CS12"/>
+    <mergeCell ref="CT10:CT12"/>
+    <mergeCell ref="CU10:CU12"/>
+    <mergeCell ref="CV10:CV12"/>
+    <mergeCell ref="CW10:CW12"/>
+    <mergeCell ref="CX10:CX12"/>
+    <mergeCell ref="CY10:CY12"/>
+    <mergeCell ref="CG10:CG12"/>
+    <mergeCell ref="CH10:CH12"/>
+    <mergeCell ref="CI10:CI12"/>
+    <mergeCell ref="CJ10:CJ12"/>
+    <mergeCell ref="CK10:CK12"/>
+    <mergeCell ref="CM10:CM12"/>
+    <mergeCell ref="CN10:CN12"/>
+    <mergeCell ref="CO10:CO12"/>
+    <mergeCell ref="CP10:CP12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="BY10:BY12"/>
+    <mergeCell ref="BZ10:BZ12"/>
+    <mergeCell ref="CA10:CA12"/>
+    <mergeCell ref="CB10:CB12"/>
+    <mergeCell ref="CC10:CC12"/>
+    <mergeCell ref="CD10:CD12"/>
+    <mergeCell ref="CE10:CE12"/>
+    <mergeCell ref="CF10:CF12"/>
+    <mergeCell ref="CS7:CS9"/>
+    <mergeCell ref="CT7:CT9"/>
+    <mergeCell ref="CU7:CU9"/>
+    <mergeCell ref="CV7:CV9"/>
+    <mergeCell ref="CW7:CW9"/>
+    <mergeCell ref="CX7:CX9"/>
+    <mergeCell ref="CY7:CY9"/>
+    <mergeCell ref="CZ7:CZ9"/>
+    <mergeCell ref="C8:C9"/>
     <mergeCell ref="CT5:CU5"/>
     <mergeCell ref="CV5:CW5"/>
     <mergeCell ref="CX5:CX6"/>
@@ -3865,299 +3794,317 @@
     <mergeCell ref="CP7:CP9"/>
     <mergeCell ref="CQ7:CQ9"/>
     <mergeCell ref="CR7:CR9"/>
-    <mergeCell ref="CS7:CS9"/>
-    <mergeCell ref="CT7:CT9"/>
-    <mergeCell ref="CU7:CU9"/>
-    <mergeCell ref="CV7:CV9"/>
-    <mergeCell ref="CW7:CW9"/>
-    <mergeCell ref="CX7:CX9"/>
-    <mergeCell ref="CY7:CY9"/>
-    <mergeCell ref="CZ7:CZ9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="BY10:BY12"/>
-    <mergeCell ref="BZ10:BZ12"/>
-    <mergeCell ref="CA10:CA12"/>
-    <mergeCell ref="CB10:CB12"/>
-    <mergeCell ref="CC10:CC12"/>
-    <mergeCell ref="CD10:CD12"/>
-    <mergeCell ref="CE10:CE12"/>
-    <mergeCell ref="CF10:CF12"/>
-    <mergeCell ref="CG10:CG12"/>
-    <mergeCell ref="CH10:CH12"/>
-    <mergeCell ref="CI10:CI12"/>
-    <mergeCell ref="CJ10:CJ12"/>
-    <mergeCell ref="CK10:CK12"/>
-    <mergeCell ref="CM10:CM12"/>
-    <mergeCell ref="CN10:CN12"/>
-    <mergeCell ref="CO10:CO12"/>
-    <mergeCell ref="CP10:CP12"/>
-    <mergeCell ref="CQ10:CQ12"/>
-    <mergeCell ref="CR10:CR12"/>
-    <mergeCell ref="CS10:CS12"/>
-    <mergeCell ref="CT10:CT12"/>
-    <mergeCell ref="CU10:CU12"/>
-    <mergeCell ref="CV10:CV12"/>
-    <mergeCell ref="CW10:CW12"/>
-    <mergeCell ref="CX10:CX12"/>
-    <mergeCell ref="CY10:CY12"/>
-    <mergeCell ref="CZ10:CZ12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="BY13:BY15"/>
-    <mergeCell ref="BZ13:BZ15"/>
-    <mergeCell ref="CA13:CA15"/>
-    <mergeCell ref="CB13:CB15"/>
-    <mergeCell ref="CC13:CC15"/>
-    <mergeCell ref="CD13:CD15"/>
-    <mergeCell ref="CE13:CE15"/>
-    <mergeCell ref="CF13:CF15"/>
-    <mergeCell ref="CG13:CG15"/>
-    <mergeCell ref="CH13:CH15"/>
-    <mergeCell ref="CI13:CI15"/>
-    <mergeCell ref="CJ13:CJ15"/>
-    <mergeCell ref="CK13:CK15"/>
-    <mergeCell ref="CM13:CM15"/>
-    <mergeCell ref="CN13:CN15"/>
-    <mergeCell ref="CO13:CO15"/>
-    <mergeCell ref="CP13:CP15"/>
-    <mergeCell ref="CQ13:CQ15"/>
-    <mergeCell ref="CR13:CR15"/>
-    <mergeCell ref="CS13:CS15"/>
-    <mergeCell ref="CT13:CT15"/>
-    <mergeCell ref="CU13:CU15"/>
-    <mergeCell ref="CV13:CV15"/>
-    <mergeCell ref="CW13:CW15"/>
-    <mergeCell ref="CX13:CX15"/>
-    <mergeCell ref="CY13:CY15"/>
-    <mergeCell ref="CZ13:CZ15"/>
+    <mergeCell ref="CF5:CG5"/>
+    <mergeCell ref="CH5:CI5"/>
+    <mergeCell ref="CJ5:CJ6"/>
+    <mergeCell ref="CK5:CK6"/>
+    <mergeCell ref="CM5:CM6"/>
+    <mergeCell ref="CN5:CO5"/>
+    <mergeCell ref="CP5:CQ5"/>
+    <mergeCell ref="CR5:CR6"/>
+    <mergeCell ref="CS5:CS6"/>
+    <mergeCell ref="BS5:BT5"/>
+    <mergeCell ref="BU5:BU6"/>
+    <mergeCell ref="BV5:BV6"/>
+    <mergeCell ref="BW5:BW6"/>
+    <mergeCell ref="BY5:BY6"/>
+    <mergeCell ref="BZ5:CA5"/>
+    <mergeCell ref="CB5:CC5"/>
+    <mergeCell ref="CD5:CD6"/>
+    <mergeCell ref="CE5:CE6"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BH5:BH6"/>
+    <mergeCell ref="BJ5:BJ6"/>
+    <mergeCell ref="BK5:BL5"/>
+    <mergeCell ref="BM5:BN5"/>
+    <mergeCell ref="BO5:BO6"/>
+    <mergeCell ref="BP5:BP6"/>
+    <mergeCell ref="BQ5:BR5"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AS5:AS6"/>
+    <mergeCell ref="AT5:AT6"/>
+    <mergeCell ref="AV5:AV6"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="BA5:BA6"/>
+    <mergeCell ref="BB5:BB6"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AE6"/>
+    <mergeCell ref="AF5:AF6"/>
+    <mergeCell ref="AH5:AH6"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AM5:AM6"/>
+    <mergeCell ref="AN5:AN6"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AN4:AT4"/>
+    <mergeCell ref="AV4:BA4"/>
+    <mergeCell ref="BB4:BH4"/>
+    <mergeCell ref="BJ4:BO4"/>
+    <mergeCell ref="BP4:BW4"/>
+    <mergeCell ref="BY4:CD4"/>
+    <mergeCell ref="CE4:CK4"/>
+    <mergeCell ref="CM4:CR4"/>
+    <mergeCell ref="CS4:CZ4"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="AH4:AM4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="T5:T6"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AB5"/>
   </mergeCells>
   <phoneticPr fontId="10"/>
   <conditionalFormatting sqref="L7">
-    <cfRule type="expression" dxfId="52" priority="77">
+    <cfRule type="expression" dxfId="55" priority="78">
       <formula>$P7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7">
-    <cfRule type="expression" dxfId="51" priority="40">
+    <cfRule type="expression" dxfId="54" priority="41">
       <formula>$X7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK7">
-    <cfRule type="expression" dxfId="50" priority="37">
+    <cfRule type="expression" dxfId="53" priority="38">
       <formula>$AL7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL7">
-    <cfRule type="expression" dxfId="49" priority="35">
+    <cfRule type="expression" dxfId="52" priority="36">
       <formula>$AL7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN7:AT7">
-    <cfRule type="expression" dxfId="48" priority="67">
+    <cfRule type="expression" dxfId="51" priority="68">
       <formula>$AR7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM9">
-    <cfRule type="expression" dxfId="47" priority="33">
+    <cfRule type="expression" dxfId="50" priority="34">
       <formula>$P9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7:I12">
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="49" priority="48">
       <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:J12">
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="48" priority="47">
       <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:K12">
-    <cfRule type="expression" dxfId="44" priority="45">
+    <cfRule type="expression" dxfId="47" priority="46">
       <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P7">
-    <cfRule type="expression" dxfId="43" priority="44">
+    <cfRule type="expression" dxfId="46" priority="45">
       <formula>$P7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7:R9">
-    <cfRule type="expression" dxfId="41" priority="43">
+    <cfRule type="expression" dxfId="45" priority="44">
       <formula>$P7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W7:W9">
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="44" priority="42">
       <formula>$X7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X8:X9">
-    <cfRule type="expression" dxfId="39" priority="39">
+    <cfRule type="expression" dxfId="43" priority="40">
       <formula>$X8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y7:Y9">
-    <cfRule type="expression" dxfId="38" priority="38">
+    <cfRule type="expression" dxfId="42" priority="39">
       <formula>$P7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK8:AK9">
-    <cfRule type="expression" dxfId="37" priority="36">
+    <cfRule type="expression" dxfId="41" priority="37">
       <formula>$AL8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL8:AL9">
-    <cfRule type="expression" dxfId="36" priority="34">
+    <cfRule type="expression" dxfId="40" priority="35">
       <formula>$AL8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM7:AM8">
-    <cfRule type="expression" dxfId="35" priority="32">
+    <cfRule type="expression" dxfId="39" priority="33">
       <formula>$P7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7:G7 G9 G11 G13 G15">
-    <cfRule type="expression" dxfId="34" priority="71">
+    <cfRule type="expression" dxfId="38" priority="72">
       <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7 H9 H11 H13 H15">
-    <cfRule type="expression" dxfId="33" priority="8">
+    <cfRule type="expression" dxfId="37" priority="9">
       <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7 M9 M11 M13 M15">
-    <cfRule type="expression" dxfId="32" priority="28">
+    <cfRule type="expression" dxfId="36" priority="29">
       <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7 N9 N11 N13 N15">
-    <cfRule type="expression" dxfId="31" priority="6">
+    <cfRule type="expression" dxfId="35" priority="7">
       <formula>$J7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T7:V7 U8:V15">
-    <cfRule type="expression" dxfId="30" priority="75">
+    <cfRule type="expression" dxfId="34" priority="76">
       <formula>$X7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z7 AC7:AF7">
-    <cfRule type="expression" dxfId="29" priority="73">
+  <conditionalFormatting sqref="Z7 AC7:AD7 AF7">
+    <cfRule type="expression" dxfId="33" priority="74">
       <formula>$AD7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7:AB15">
-    <cfRule type="expression" dxfId="28" priority="14">
+    <cfRule type="expression" dxfId="32" priority="15">
       <formula>$X7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH7:AJ7 AI8:AJ15">
-    <cfRule type="expression" dxfId="27" priority="68">
+    <cfRule type="expression" dxfId="31" priority="69">
       <formula>$AL7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV7:BA7 AX8:AX15">
-    <cfRule type="expression" dxfId="26" priority="62">
+    <cfRule type="expression" dxfId="30" priority="63">
       <formula>$AZ7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB7:BH7 BC8:BC15">
-    <cfRule type="expression" dxfId="25" priority="61">
+    <cfRule type="expression" dxfId="29" priority="62">
       <formula>$BF7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ7:BO7 BL8:BL15">
-    <cfRule type="expression" dxfId="24" priority="56">
+    <cfRule type="expression" dxfId="28" priority="57">
       <formula>$BN7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP7:BW7 BQ8:BQ15">
-    <cfRule type="expression" dxfId="23" priority="55">
+    <cfRule type="expression" dxfId="27" priority="56">
       <formula>$BT7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F15 I13:K15 F8:G8 G10 G12 G14">
-    <cfRule type="expression" dxfId="22" priority="78">
+    <cfRule type="expression" dxfId="26" priority="79">
       <formula>$J8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8 H10 H12 H14">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="25" priority="10">
       <formula>$J8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L15 O10:R15">
-    <cfRule type="expression" dxfId="20" priority="76">
+    <cfRule type="expression" dxfId="24" priority="77">
       <formula>$P8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8 M10 M12 M14">
-    <cfRule type="expression" dxfId="19" priority="7">
+    <cfRule type="expression" dxfId="23" priority="8">
       <formula>$J8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8 N10 N12 N14">
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>$J8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T8:T15 W10:Y15">
-    <cfRule type="expression" dxfId="17" priority="70">
+    <cfRule type="expression" dxfId="21" priority="71">
       <formula>$X8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z8:Z15 AC8:AF15">
-    <cfRule type="expression" dxfId="16" priority="69">
+    <cfRule type="expression" dxfId="20" priority="70">
       <formula>$AD8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH8:AH15 AK10:AM15">
-    <cfRule type="expression" dxfId="15" priority="64">
+    <cfRule type="expression" dxfId="19" priority="65">
       <formula>$AL8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN8:AT15">
-    <cfRule type="expression" dxfId="14" priority="63">
+    <cfRule type="expression" dxfId="18" priority="64">
       <formula>$AR8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV8:AW15 AY8:BA15">
-    <cfRule type="expression" dxfId="13" priority="58">
+    <cfRule type="expression" dxfId="17" priority="59">
       <formula>$AZ8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB8:BB15 BD8:BH15">
-    <cfRule type="expression" dxfId="12" priority="57">
+    <cfRule type="expression" dxfId="16" priority="58">
       <formula>$BF8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ8:BK15 BM8:BO15">
-    <cfRule type="expression" dxfId="11" priority="50">
+    <cfRule type="expression" dxfId="15" priority="51">
       <formula>$BN8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP8:BP15 BR8:BW15">
-    <cfRule type="expression" dxfId="10" priority="49">
+    <cfRule type="expression" dxfId="14" priority="50">
       <formula>$BT8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O7:O9">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>$P7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P8">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>$P8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$P9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q7:Q9">
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>$P7&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$P7&lt;&gt;""</formula>
     </cfRule>
@@ -4175,9 +4122,9 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
   <sheetData>
-    <row r="5">
+    <row r="5" spans="4:5">
       <c r="D5" s="1" t="s">
         <v>47</v>
       </c>
@@ -4185,19 +4132,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="4:5">
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="4:5">
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="4:5">
       <c r="D8" s="1" t="s">
         <v>49</v>
       </c>
@@ -4205,19 +4152,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="4:5">
       <c r="D9" s="3"/>
       <c r="E9" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="4:5">
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="4:5">
       <c r="D11" s="1" t="s">
         <v>50</v>
       </c>
@@ -4225,13 +4172,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="4:5">
       <c r="D12" s="3"/>
       <c r="E12" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="4:5">
       <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
         <v>46</v>
@@ -4240,47 +4187,47 @@
   </sheetData>
   <phoneticPr fontId="10"/>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>$H5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>$H6&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$H7&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>$H8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$H9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$H10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$H11&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$H12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$H13&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>